<commit_message>
eBGP between first CE-PE's + interface addresses
-The Documentation file was renamed
-The Addressing chart was changed, so the private LAN's of the CE are with /24 mask
-Established eBGP peering between the first half of CE's - PE's
-Idle-PC's are recomputed in order to use less resources
-Added description to interfaces
-Added Cisco vIOS Image to the folder
</commit_message>
<xml_diff>
--- a/Addressing Chart.xlsx
+++ b/Addressing Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Dimplomna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Diplomna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E27930-3D24-4074-B4EB-56FE6653DB48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99CF479-661B-4963-90A3-240926908E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="0" windowWidth="14430" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
+    <workbookView xWindow="105" yWindow="210" windowWidth="14430" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="86">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>122.112.1.1</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
   </si>
 </sst>
 </file>
@@ -792,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60363D47-2DAE-4CE4-B50C-02B700C9D128}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,12 +809,12 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -825,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -836,10 +839,10 @@
         <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -851,7 +854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -863,7 +866,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
@@ -874,10 +877,10 @@
         <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -888,8 +891,11 @@
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -901,7 +907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
@@ -915,7 +921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
@@ -927,7 +933,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16"/>
       <c r="C11" s="2" t="s">
         <v>7</v>
@@ -939,7 +945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
         <v>21</v>
@@ -951,7 +957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
       <c r="C13" s="2" t="s">
         <v>22</v>
@@ -963,7 +969,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>10</v>
       </c>
@@ -977,7 +983,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="16"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -989,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16"/>
       <c r="C16" s="2" t="s">
         <v>7</v>
@@ -1484,7 +1490,7 @@
         <v>39</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1522,7 +1528,7 @@
         <v>38</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
eBGP finished, IS-IS IGP first half, addressing done
-Every PE and CE are with configured with eBGP
-The first half of the backbone has IS-IS set up and working
-Addressing chart changed due to a mistake
-All the used interfaces are configured with IPv4
-Added some required fields in Documentation
</commit_message>
<xml_diff>
--- a/Addressing Chart.xlsx
+++ b/Addressing Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Diplomna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99CF479-661B-4963-90A3-240926908E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55663457-39DB-4092-BE3F-0124131972FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="210" windowWidth="14430" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
+    <workbookView xWindow="-1050" yWindow="330" windowWidth="14430" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="87">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>122.0.13.2</t>
   </si>
 </sst>
 </file>
@@ -321,7 +324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +346,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -470,6 +479,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60363D47-2DAE-4CE4-B50C-02B700C9D128}">
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,61 +1062,61 @@
     </row>
     <row r="20" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="16"/>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1199,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
MPLS + iBGP + Route reflection
-Slight changes to the documentation
-All ISP routers now have enabled MPLS
-PE's have iBGP to RR's
-PE's set as route reflector clients
-New changes to style
-New connections and thus IP addresses
</commit_message>
<xml_diff>
--- a/Addressing Chart.xlsx
+++ b/Addressing Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Diplomna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55663457-39DB-4092-BE3F-0124131972FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6319FC9-D323-4C02-9E0C-0CFFBC60DF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1050" yWindow="330" windowWidth="14430" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
+    <workbookView xWindow="0" yWindow="225" windowWidth="12405" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>122.0.13.2</t>
+  </si>
+  <si>
+    <t>122.0.36.1</t>
+  </si>
+  <si>
+    <t>122.0.16.1</t>
+  </si>
+  <si>
+    <t>122.0.16.2</t>
+  </si>
+  <si>
+    <t>122.0.36.2</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60363D47-2DAE-4CE4-B50C-02B700C9D128}">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,10 +1099,10 @@
     <row r="22" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
       <c r="C22" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>24</v>
@@ -1099,60 +1111,60 @@
     <row r="23" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
       <c r="C23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="16"/>
+      <c r="C24" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D24" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15"/>
-      <c r="C24" s="17" t="s">
+      <c r="E24" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D25" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
+      <c r="E25" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>24</v>
@@ -1161,60 +1173,60 @@
     <row r="28" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="16"/>
       <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="16"/>
+      <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15"/>
-      <c r="C29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15"/>
+      <c r="C30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
+      <c r="E30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="16"/>
       <c r="C32" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>24</v>
@@ -1223,10 +1235,10 @@
     <row r="33" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="16"/>
       <c r="C33" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>24</v>
@@ -1235,110 +1247,108 @@
     <row r="34" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="16"/>
       <c r="C34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="16"/>
+      <c r="C35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="15"/>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="16"/>
+      <c r="C36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="15"/>
+      <c r="C37" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="14" t="s">
+      <c r="E37" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="16"/>
-      <c r="C37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="16"/>
       <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="16"/>
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="16"/>
+      <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="15"/>
-      <c r="C40" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E41" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="15"/>
       <c r="C42" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>24</v>
@@ -1346,113 +1356,113 @@
     </row>
     <row r="43" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="15"/>
-      <c r="C44" s="2" t="s">
+      <c r="B44" s="16"/>
+      <c r="C44" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="15"/>
+      <c r="C45" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="16"/>
-      <c r="C46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="16"/>
-      <c r="C47" s="2" t="s">
-        <v>7</v>
+      <c r="C47" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="16"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="15"/>
-      <c r="C49" s="2" t="s">
-        <v>22</v>
+      <c r="B49" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>25</v>
+      <c r="B50" s="16"/>
+      <c r="C50" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="16"/>
       <c r="C51" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>24</v>
@@ -1461,138 +1471,164 @@
     <row r="52" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="16"/>
       <c r="C52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="15"/>
+      <c r="C53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="16"/>
+      <c r="C55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="16"/>
+      <c r="C56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="16"/>
-      <c r="C53" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="16"/>
+      <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="15"/>
-      <c r="C54" s="2" t="s">
+      <c r="E57" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="15"/>
+      <c r="C58" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="8" t="s">
+      <c r="E58" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="9"/>
-      <c r="C56" s="2" t="s">
+    <row r="60" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="9"/>
+      <c r="C60" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="10"/>
-      <c r="C57" s="2" t="s">
+      <c r="E60" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="10"/>
+      <c r="C61" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="11" t="s">
+      <c r="E61" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D62" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="12"/>
-      <c r="C59" s="2" t="s">
+    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="12"/>
+      <c r="C63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="13"/>
-      <c r="C60" s="2" t="s">
+      <c r="E63" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="13"/>
+      <c r="C64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
+      <c r="E64" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
@@ -1738,21 +1774,45 @@
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
     </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="B49:B53"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B30:B35"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B26:B30"/>
     <mergeCell ref="B9:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Documentation + Addressing chart Rework
-Chapter 1 done
</commit_message>
<xml_diff>
--- a/Addressing Chart.xlsx
+++ b/Addressing Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Diplomna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6319FC9-D323-4C02-9E0C-0CFFBC60DF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFC31DA-DD9A-4D79-A352-60A597CD27FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="225" windowWidth="12405" windowHeight="15375" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE359840-CB24-4AF2-8F89-D005508FA20B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="91">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +364,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -464,6 +470,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -487,16 +499,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -822,26 +837,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60363D47-2DAE-4CE4-B50C-02B700C9D128}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:W92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="22.7109375" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -854,9 +881,45 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -868,9 +931,45 @@
       <c r="E3" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9"/>
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
@@ -880,9 +979,39 @@
       <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="17"/>
+      <c r="U4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
@@ -892,9 +1021,39 @@
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="17"/>
+      <c r="U5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -906,9 +1065,41 @@
       <c r="E6" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
+      <c r="H6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="17"/>
+      <c r="U6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="14"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
@@ -918,12 +1109,39 @@
       <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="18"/>
+      <c r="O7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" s="17"/>
+      <c r="U7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15"/>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
@@ -933,9 +1151,41 @@
       <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T8" s="17"/>
+      <c r="U8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -947,9 +1197,41 @@
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
+      <c r="H9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="17"/>
+      <c r="O9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T9" s="18"/>
+      <c r="U9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
@@ -959,9 +1241,41 @@
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="17"/>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
@@ -971,9 +1285,39 @@
       <c r="E11" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="17"/>
+      <c r="O11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T11" s="17"/>
+      <c r="U11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="17"/>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
@@ -983,9 +1327,41 @@
       <c r="E12" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
+      <c r="H12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="18"/>
+      <c r="O12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12" s="17"/>
+      <c r="U12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="18"/>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
@@ -995,9 +1371,41 @@
       <c r="E13" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T13" s="17"/>
+      <c r="U13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1009,9 +1417,39 @@
       <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="17"/>
+      <c r="O14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T14" s="18"/>
+      <c r="U14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1021,9 +1459,31 @@
       <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17"/>
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1033,9 +1493,41 @@
       <c r="E16" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
+      <c r="H16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="17"/>
+      <c r="O16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="17"/>
+      <c r="U16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="17"/>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1045,9 +1537,41 @@
       <c r="E17" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
+      <c r="H17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="18"/>
+      <c r="O17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="17"/>
+      <c r="U17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1057,9 +1581,41 @@
       <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="H18" s="17"/>
+      <c r="I18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T18" s="17"/>
+      <c r="U18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1071,81 +1627,235 @@
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="H19" s="18"/>
+      <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="17"/>
+      <c r="O19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="P19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T19" s="17"/>
+      <c r="U19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17" t="s">
+      <c r="E20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="17"/>
+      <c r="O20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="P20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" s="17"/>
+      <c r="U20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17" t="s">
+      <c r="E21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="J21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="17"/>
+      <c r="O21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="18"/>
+      <c r="U21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
+      <c r="C22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="17" t="s">
+      <c r="E22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" s="18"/>
+      <c r="O22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="P22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="17"/>
+      <c r="C23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="16"/>
-      <c r="C24" s="17" t="s">
+      <c r="E23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T23" s="17"/>
+      <c r="U23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15"/>
-      <c r="C25" s="17" t="s">
+      <c r="E24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T24" s="17"/>
+      <c r="U24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="18"/>
+      <c r="C25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
+      <c r="E25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T25" s="17"/>
+      <c r="U25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1157,9 +1867,19 @@
       <c r="E26" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="16"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="17"/>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1170,8 +1890,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
+    <row r="28" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="17"/>
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
@@ -1182,8 +1902,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
+    <row r="29" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
       <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1194,8 +1914,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15"/>
+    <row r="30" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="18"/>
       <c r="C30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1206,8 +1926,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1220,8 +1940,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="16"/>
+    <row r="32" spans="2:23" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="17"/>
       <c r="C32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1953,7 @@
       </c>
     </row>
     <row r="33" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="16"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1965,7 @@
       </c>
     </row>
     <row r="34" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
@@ -1257,7 +1977,7 @@
       </c>
     </row>
     <row r="35" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="16"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="2" t="s">
         <v>22</v>
       </c>
@@ -1269,7 +1989,7 @@
       </c>
     </row>
     <row r="36" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="16"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="2" t="s">
         <v>28</v>
       </c>
@@ -1281,7 +2001,7 @@
       </c>
     </row>
     <row r="37" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="15"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="2" t="s">
         <v>23</v>
       </c>
@@ -1293,7 +2013,7 @@
       </c>
     </row>
     <row r="38" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -1307,7 +2027,7 @@
       </c>
     </row>
     <row r="39" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="16"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +2039,7 @@
       </c>
     </row>
     <row r="40" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="16"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
@@ -1331,7 +2051,7 @@
       </c>
     </row>
     <row r="41" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="16"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
@@ -1343,7 +2063,7 @@
       </c>
     </row>
     <row r="42" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="15"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="2" t="s">
         <v>22</v>
       </c>
@@ -1355,7 +2075,7 @@
       </c>
     </row>
     <row r="43" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -1369,8 +2089,8 @@
       </c>
     </row>
     <row r="44" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="16"/>
-      <c r="C44" s="17" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -1381,7 +2101,7 @@
       </c>
     </row>
     <row r="45" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="15"/>
+      <c r="B45" s="18"/>
       <c r="C45" s="2" t="s">
         <v>23</v>
       </c>
@@ -1393,7 +2113,7 @@
       </c>
     </row>
     <row r="46" spans="2:5" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -1407,8 +2127,8 @@
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="16"/>
-      <c r="C47" s="17" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -1419,7 +2139,7 @@
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="15"/>
+      <c r="B48" s="18"/>
       <c r="C48" s="2" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +2151,7 @@
       </c>
     </row>
     <row r="49" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -1445,7 +2165,7 @@
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="16"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="2" t="s">
         <v>6</v>
       </c>
@@ -1457,7 +2177,7 @@
       </c>
     </row>
     <row r="51" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="16"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="2" t="s">
         <v>7</v>
       </c>
@@ -1469,7 +2189,7 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="16"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +2201,7 @@
       </c>
     </row>
     <row r="53" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="15"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="2" t="s">
         <v>22</v>
       </c>
@@ -1493,7 +2213,7 @@
       </c>
     </row>
     <row r="54" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -1507,7 +2227,7 @@
       </c>
     </row>
     <row r="55" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="16"/>
+      <c r="B55" s="17"/>
       <c r="C55" s="2" t="s">
         <v>6</v>
       </c>
@@ -1519,7 +2239,7 @@
       </c>
     </row>
     <row r="56" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="16"/>
+      <c r="B56" s="17"/>
       <c r="C56" s="2" t="s">
         <v>7</v>
       </c>
@@ -1531,7 +2251,7 @@
       </c>
     </row>
     <row r="57" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="16"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
@@ -1543,7 +2263,7 @@
       </c>
     </row>
     <row r="58" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="15"/>
+      <c r="B58" s="18"/>
       <c r="C58" s="2" t="s">
         <v>22</v>
       </c>
@@ -1555,7 +2275,7 @@
       </c>
     </row>
     <row r="59" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C59" s="7" t="s">
@@ -1569,7 +2289,7 @@
       </c>
     </row>
     <row r="60" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="9"/>
+      <c r="B60" s="11"/>
       <c r="C60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1581,7 +2301,7 @@
       </c>
     </row>
     <row r="61" spans="2:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="10"/>
+      <c r="B61" s="12"/>
       <c r="C61" s="2" t="s">
         <v>7</v>
       </c>
@@ -1592,8 +2312,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="11" t="s">
+    <row r="62" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -1606,8 +2326,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="12"/>
+    <row r="63" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="14"/>
       <c r="C63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1618,8 +2338,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="13"/>
+    <row r="64" spans="2:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="15"/>
       <c r="C64" s="2" t="s">
         <v>7</v>
       </c>
@@ -1799,7 +2519,26 @@
       <c r="E92" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="28">
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="N18:N22"/>
+    <mergeCell ref="T3:T9"/>
+    <mergeCell ref="T10:T14"/>
+    <mergeCell ref="T15:T21"/>
+    <mergeCell ref="T22:T26"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="N8:N12"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B9:B13"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="B31:B37"/>
@@ -1809,11 +2548,6 @@
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="B54:B58"/>
     <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B9:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>